<commit_message>
Graph and README added
</commit_message>
<xml_diff>
--- a/Building Data/FDC_1min_01DEC2022.xlsx
+++ b/Building Data/FDC_1min_01DEC2022.xlsx
@@ -5,15 +5,15 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lore3652\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ustugrid\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5707B5C-AE34-4669-8855-99700D1DCAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1D9D29-A85F-462B-8D44-A1CEFCAE8881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ReadMe" sheetId="8" r:id="rId1"/>
+    <sheet name="README" sheetId="8" r:id="rId1"/>
     <sheet name="FDC_1Min_2022121" sheetId="1" r:id="rId2"/>
     <sheet name="Power Output" sheetId="5" r:id="rId3"/>
     <sheet name="Line to Line Voltage" sheetId="6" r:id="rId4"/>
@@ -65,14 +65,14 @@
     <t>This project was made possible in whole or in part by a grant from the Minnesota Department of Commerce through the Minnesota Renewable Development Account, which is financed by Xcel Energy ratepayers. CMR sincerely thanks the Minnesota Department of Commerce, the Minnesota State Legislature, and Xcel Energy for their invaluable support in establishing the Center for Microgrid Research. Their contributions have been instrumental in advancing microgrid research and this data collection.</t>
   </si>
   <si>
-    <t>Data Title: FDC One Minute Data 01DEC2022</t>
+    <t>Data Title: FDC_1min_01DEC2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,12 +203,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -555,14 +549,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1082,20 +1075,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFB59A0-FEFC-483A-B03B-9CCE7F612849}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11310337-C2DB-4E11-9BA3-A9C7DE97EF7C}">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.7109375" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1119,7 +1112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1135,7 +1128,7 @@
   <dimension ref="A1:H1441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>